<commit_message>
Them proc xoa nhan vien
</commit_message>
<xml_diff>
--- a/Phân công công việc bài 1.xlsx
+++ b/Phân công công việc bài 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>STT</t>
   </si>
@@ -118,11 +118,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -326,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -394,6 +415,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -702,18 +744,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G8:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" customWidth="1"/>
-    <col min="11" max="11" width="30.140625" customWidth="1"/>
-    <col min="12" max="12" width="48.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.625" customWidth="1"/>
+    <col min="8" max="8" width="25.125" customWidth="1"/>
+    <col min="9" max="9" width="25.25" customWidth="1"/>
+    <col min="10" max="10" width="33.25" customWidth="1"/>
+    <col min="11" max="11" width="30.125" customWidth="1"/>
+    <col min="12" max="12" width="48.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -788,7 +830,7 @@
       <c r="J12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="27" t="s">
         <v>12</v>
       </c>
       <c r="L12" s="12" t="s">
@@ -827,7 +869,7 @@
       <c r="K14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="30" t="s">
         <v>17</v>
       </c>
     </row>
@@ -839,10 +881,12 @@
         <v>18</v>
       </c>
       <c r="I15" s="11"/>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="11"/>
+      <c r="K15" s="32" t="s">
+        <v>12</v>
+      </c>
       <c r="L15" s="12" t="s">
         <v>20</v>
       </c>
@@ -953,10 +997,10 @@
       </c>
     </row>
     <row r="31" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="H31" s="23">
+      <c r="H31" s="28">
         <v>1.3</v>
       </c>
-      <c r="I31" s="23" t="s">
+      <c r="I31" s="28" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1009,10 +1053,10 @@
       </c>
     </row>
     <row r="38" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H38" s="26">
+      <c r="H38" s="29">
         <v>3.4</v>
       </c>
-      <c r="I38" s="26" t="s">
+      <c r="I38" s="29" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1025,10 +1069,10 @@
       </c>
     </row>
     <row r="40" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H40" s="24">
+      <c r="H40" s="31">
         <v>4.3</v>
       </c>
-      <c r="I40" s="24" t="s">
+      <c r="I40" s="31" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>